<commit_message>
Fix Obs avoidance and Refactor v2
</commit_message>
<xml_diff>
--- a/Assets/Roadmap v2.xlsx
+++ b/Assets/Roadmap v2.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\RTS-3D-Project-v2\Assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -105,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +246,7 @@
           <xdr:col>9</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>42</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -264,7 +259,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -272,17 +267,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -316,7 +300,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -324,17 +308,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -388,7 +361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,7 +396,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +608,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed select object and additional click behavior
Chọn 1 obj -> huỷ chọn ~ obj còn lại
Fixed khi chọn đối tượng thì không set pointer
</commit_message>
<xml_diff>
--- a/Assets/Roadmap v2.xlsx
+++ b/Assets/Roadmap v2.xlsx
@@ -160,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,6 +207,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,10 +722,10 @@
       <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -743,6 +746,7 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
FixBug after mesh 21/10/2018
</commit_message>
<xml_diff>
--- a/Assets/Roadmap v2.xlsx
+++ b/Assets/Roadmap v2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\RTS-3D-Project-v2\Assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>AI theo nhóm và riêng lẻ</t>
   </si>
@@ -84,9 +89,6 @@
     <t>Test và sửa lỗi</t>
   </si>
   <si>
-    <t>Thứ 7 - 27-10-2018</t>
-  </si>
-  <si>
     <t>Điều khiển cơ bản</t>
   </si>
   <si>
@@ -94,12 +96,18 @@
   </si>
   <si>
     <t xml:space="preserve">Mini Map </t>
+  </si>
+  <si>
+    <t>Thứ 3 - 6-11-2018</t>
+  </si>
+  <si>
+    <t>Thứ 3 - 30-10-2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,6 +218,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -261,7 +272,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -269,6 +280,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -302,7 +324,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -310,6 +332,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -363,7 +396,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,7 +431,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,9 +660,9 @@
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -649,7 +682,7 @@
       </c>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,17 +704,14 @@
       <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -691,17 +721,17 @@
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="18"/>
@@ -713,9 +743,9 @@
       <c r="I4" s="8"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="5" t="s">
@@ -731,12 +761,17 @@
         <v>18</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J5" s="15"/>
+      <c r="K5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="C5:D5"/>

</xml_diff>